<commit_message>
fixed problem with unknowingly recursively calling simp_express
</commit_message>
<xml_diff>
--- a/FindDuplicates/PascalParseTable.xlsx
+++ b/FindDuplicates/PascalParseTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\FindDuplicates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin\home\chris\CompilerConstruction\FindDuplicates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4E72B7-880F-4711-9A89-1D5C5BA3F3A2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B48783-6CFE-418F-B850-88C8E7B83FA2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="16335" windowHeight="10830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="115">
   <si>
     <t>prgrm</t>
   </si>
@@ -667,9 +667,6 @@
   </si>
   <si>
     <t>cmpnd_stmnt .</t>
-  </si>
-  <si>
-    <t>term simp_express</t>
   </si>
   <si>
     <t>expressp</t>
@@ -1354,9 +1351,9 @@
   </sheetPr>
   <dimension ref="A1:AI41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AF39" sqref="AF39"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1482,10 +1479,10 @@
         <v>49</v>
       </c>
       <c r="AG1" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH1" s="14" t="s">
         <v>114</v>
-      </c>
-      <c r="AH1" s="14" t="s">
-        <v>115</v>
       </c>
       <c r="AI1" s="10" t="s">
         <v>52</v>
@@ -1496,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>50</v>
@@ -1600,28 +1597,28 @@
     </row>
     <row r="3" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>50</v>
@@ -1707,7 +1704,7 @@
     </row>
     <row r="4" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>50</v>
@@ -1820,7 +1817,7 @@
         <v>50</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>50</v>
@@ -1921,7 +1918,7 @@
     </row>
     <row r="6" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>50</v>
@@ -1939,7 +1936,7 @@
         <v>50</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>50</v>
@@ -2049,7 +2046,7 @@
         <v>50</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>50</v>
@@ -2135,7 +2132,7 @@
     </row>
     <row r="8" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>50</v>
@@ -2156,7 +2153,7 @@
         <v>50</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>50</v>
@@ -2510,7 +2507,7 @@
         <v>50</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T11" s="3" t="s">
         <v>50</v>
@@ -2563,7 +2560,7 @@
     </row>
     <row r="12" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>50</v>
@@ -2617,7 +2614,7 @@
         <v>50</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T12" s="11" t="s">
         <v>53</v>
@@ -2724,7 +2721,7 @@
         <v>50</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="T13" s="3" t="s">
         <v>50</v>
@@ -2777,28 +2774,28 @@
     </row>
     <row r="14" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>50</v>
@@ -2884,7 +2881,7 @@
     </row>
     <row r="15" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>50</v>
@@ -3045,7 +3042,7 @@
         <v>50</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="T16" s="3" t="s">
         <v>50</v>
@@ -3098,7 +3095,7 @@
     </row>
     <row r="17" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>50</v>
@@ -3318,7 +3315,7 @@
         <v>50</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>50</v>
@@ -3419,7 +3416,7 @@
     </row>
     <row r="20" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>50</v>
@@ -3434,7 +3431,7 @@
         <v>53</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>50</v>
@@ -3583,7 +3580,7 @@
         <v>50</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U21" s="3" t="s">
         <v>50</v>
@@ -3633,7 +3630,7 @@
     </row>
     <row r="22" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>50</v>
@@ -3853,7 +3850,7 @@
         <v>50</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>50</v>
@@ -3904,7 +3901,7 @@
         <v>50</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U24" s="3" t="s">
         <v>50</v>
@@ -3913,7 +3910,7 @@
         <v>50</v>
       </c>
       <c r="W24" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="X24" s="3" t="s">
         <v>50</v>
@@ -3922,13 +3919,13 @@
         <v>50</v>
       </c>
       <c r="Z24" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AA24" s="3" t="s">
         <v>50</v>
       </c>
       <c r="AB24" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AC24" s="3" t="s">
         <v>50</v>
@@ -3954,7 +3951,7 @@
     </row>
     <row r="25" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>50</v>
@@ -4127,7 +4124,7 @@
         <v>50</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="X26" s="3" t="s">
         <v>50</v>
@@ -4174,7 +4171,7 @@
         <v>50</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>50</v>
@@ -4275,7 +4272,7 @@
     </row>
     <row r="28" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>50</v>
@@ -4463,7 +4460,7 @@
         <v>50</v>
       </c>
       <c r="AB29" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AC29" s="3" t="s">
         <v>50</v>
@@ -4489,7 +4486,7 @@
     </row>
     <row r="30" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>50</v>
@@ -4602,10 +4599,10 @@
         <v>50</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>50</v>
@@ -4641,7 +4638,7 @@
         <v>50</v>
       </c>
       <c r="P31" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q31" s="3" t="s">
         <v>50</v>
@@ -4689,13 +4686,13 @@
         <v>50</v>
       </c>
       <c r="AF31" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AG31" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AH31" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AI31" s="3" t="s">
         <v>50</v>
@@ -4703,7 +4700,7 @@
     </row>
     <row r="32" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>50</v>
@@ -4721,7 +4718,7 @@
         <v>50</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>50</v>
@@ -4816,10 +4813,10 @@
         <v>50</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>50</v>
@@ -4855,7 +4852,7 @@
         <v>50</v>
       </c>
       <c r="P33" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q33" s="3" t="s">
         <v>50</v>
@@ -4903,13 +4900,13 @@
         <v>50</v>
       </c>
       <c r="AF33" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AG33" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AH33" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AI33" s="3" t="s">
         <v>50</v>
@@ -4917,7 +4914,7 @@
     </row>
     <row r="34" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>50</v>
@@ -5030,10 +5027,10 @@
         <v>50</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>50</v>
@@ -5069,61 +5066,61 @@
         <v>50</v>
       </c>
       <c r="P35" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="S35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="U35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="V35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="W35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="X35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF35" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG35" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="Q35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="R35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="S35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="T35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="U35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="V35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="W35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="X35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF35" s="4" t="s">
+      <c r="AH35" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="AG35" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="AH35" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="AI35" s="3" t="s">
         <v>50</v>
@@ -5131,7 +5128,7 @@
     </row>
     <row r="36" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>50</v>
@@ -5218,7 +5215,7 @@
         <v>53</v>
       </c>
       <c r="AD36" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AE36" s="3" t="s">
         <v>50</v>
@@ -5244,10 +5241,10 @@
         <v>50</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>50</v>
@@ -5283,7 +5280,7 @@
         <v>50</v>
       </c>
       <c r="P37" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q37" s="3" t="s">
         <v>50</v>
@@ -5331,7 +5328,7 @@
         <v>50</v>
       </c>
       <c r="AF37" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AG37" s="3" t="s">
         <v>50</v>
@@ -5345,7 +5342,7 @@
     </row>
     <row r="38" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>50</v>
@@ -5435,7 +5432,7 @@
         <v>53</v>
       </c>
       <c r="AE38" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AF38" s="3" t="s">
         <v>50</v>
@@ -5458,7 +5455,7 @@
         <v>50</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>67</v>
@@ -5559,7 +5556,7 @@
     </row>
     <row r="40" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>50</v>
@@ -5762,10 +5759,10 @@
         <v>50</v>
       </c>
       <c r="AG41" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH41" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="AH41" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="AI41" s="3" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
fixed subprogram declaration, need to test more complex program
</commit_message>
<xml_diff>
--- a/FindDuplicates/PascalParseTable.xlsx
+++ b/FindDuplicates/PascalParseTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin\home\chris\CompilerConstruction\FindDuplicates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B48783-6CFE-418F-B850-88C8E7B83FA2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B99BD8-51A6-4138-8447-0D1DE7744379}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="16335" windowHeight="10830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -711,9 +711,6 @@
     <t>subprgrm_declsp</t>
   </si>
   <si>
-    <t>subprgrm_decl subprgrm_declp</t>
-  </si>
-  <si>
     <t>subprgrm_declp</t>
   </si>
   <si>
@@ -920,6 +917,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>subprgrm_head subprgrm_declp</t>
   </si>
 </sst>
 </file>
@@ -1351,9 +1351,9 @@
   </sheetPr>
   <dimension ref="A1:AI41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1479,10 +1479,10 @@
         <v>49</v>
       </c>
       <c r="AG1" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="AH1" s="14" t="s">
         <v>113</v>
-      </c>
-      <c r="AH1" s="14" t="s">
-        <v>114</v>
       </c>
       <c r="AI1" s="10" t="s">
         <v>52</v>
@@ -2507,7 +2507,7 @@
         <v>50</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="T11" s="3" t="s">
         <v>50</v>
@@ -2614,7 +2614,7 @@
         <v>50</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="T12" s="11" t="s">
         <v>53</v>
@@ -2721,7 +2721,7 @@
         <v>50</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="T13" s="3" t="s">
         <v>50</v>
@@ -2774,28 +2774,28 @@
     </row>
     <row r="14" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>50</v>
@@ -2881,7 +2881,7 @@
     </row>
     <row r="15" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>50</v>
@@ -3042,7 +3042,7 @@
         <v>50</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="T16" s="3" t="s">
         <v>50</v>
@@ -3095,7 +3095,7 @@
     </row>
     <row r="17" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>50</v>
@@ -3315,7 +3315,7 @@
         <v>50</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>50</v>
@@ -3416,7 +3416,7 @@
     </row>
     <row r="20" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>50</v>
@@ -3431,7 +3431,7 @@
         <v>53</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>50</v>
@@ -3580,7 +3580,7 @@
         <v>50</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="U21" s="3" t="s">
         <v>50</v>
@@ -3630,7 +3630,7 @@
     </row>
     <row r="22" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>50</v>
@@ -3850,7 +3850,7 @@
         <v>50</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>50</v>
@@ -3901,7 +3901,7 @@
         <v>50</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U24" s="3" t="s">
         <v>50</v>
@@ -3910,7 +3910,7 @@
         <v>50</v>
       </c>
       <c r="W24" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X24" s="3" t="s">
         <v>50</v>
@@ -3919,13 +3919,13 @@
         <v>50</v>
       </c>
       <c r="Z24" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AA24" s="3" t="s">
         <v>50</v>
       </c>
       <c r="AB24" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AC24" s="3" t="s">
         <v>50</v>
@@ -3951,7 +3951,7 @@
     </row>
     <row r="25" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>50</v>
@@ -4124,7 +4124,7 @@
         <v>50</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="X26" s="3" t="s">
         <v>50</v>
@@ -4171,7 +4171,7 @@
         <v>50</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>50</v>
@@ -4272,7 +4272,7 @@
     </row>
     <row r="28" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>50</v>
@@ -4460,7 +4460,7 @@
         <v>50</v>
       </c>
       <c r="AB29" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC29" s="3" t="s">
         <v>50</v>
@@ -4486,7 +4486,7 @@
     </row>
     <row r="30" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>50</v>
@@ -4599,10 +4599,10 @@
         <v>50</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>50</v>
@@ -4638,7 +4638,7 @@
         <v>50</v>
       </c>
       <c r="P31" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q31" s="3" t="s">
         <v>50</v>
@@ -4686,13 +4686,13 @@
         <v>50</v>
       </c>
       <c r="AF31" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AG31" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AH31" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI31" s="3" t="s">
         <v>50</v>
@@ -4700,7 +4700,7 @@
     </row>
     <row r="32" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>50</v>
@@ -4718,7 +4718,7 @@
         <v>50</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>50</v>
@@ -4813,10 +4813,10 @@
         <v>50</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>50</v>
@@ -4852,7 +4852,7 @@
         <v>50</v>
       </c>
       <c r="P33" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q33" s="3" t="s">
         <v>50</v>
@@ -4900,13 +4900,13 @@
         <v>50</v>
       </c>
       <c r="AF33" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AG33" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AH33" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AI33" s="3" t="s">
         <v>50</v>
@@ -5027,100 +5027,100 @@
         <v>50</v>
       </c>
       <c r="C35" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="N35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P35" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="S35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="U35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="V35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="W35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="X35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF35" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="AG35" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="AH35" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="K35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="L35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="N35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="O35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P35" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="R35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="S35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="T35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="U35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="V35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="W35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="X35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF35" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="AG35" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="AH35" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="AI35" s="3" t="s">
         <v>50</v>
@@ -5215,7 +5215,7 @@
         <v>53</v>
       </c>
       <c r="AD36" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AE36" s="3" t="s">
         <v>50</v>
@@ -5241,10 +5241,10 @@
         <v>50</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>50</v>
@@ -5280,7 +5280,7 @@
         <v>50</v>
       </c>
       <c r="P37" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q37" s="3" t="s">
         <v>50</v>
@@ -5328,7 +5328,7 @@
         <v>50</v>
       </c>
       <c r="AF37" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AG37" s="3" t="s">
         <v>50</v>
@@ -5432,7 +5432,7 @@
         <v>53</v>
       </c>
       <c r="AE38" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AF38" s="3" t="s">
         <v>50</v>
@@ -5455,7 +5455,7 @@
         <v>50</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>67</v>
@@ -5759,10 +5759,10 @@
         <v>50</v>
       </c>
       <c r="AG41" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AH41" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="AH41" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="AI41" s="3" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
fixed else error, turned out to be problem with expressp not breaking for else
</commit_message>
<xml_diff>
--- a/FindDuplicates/PascalParseTable.xlsx
+++ b/FindDuplicates/PascalParseTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin\home\chris\CompilerConstruction\FindDuplicates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B99BD8-51A6-4138-8447-0D1DE7744379}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3AA629-5FAF-48C1-ABBB-9903339E3990}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="16335" windowHeight="10830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1351,9 +1351,9 @@
   </sheetPr>
   <dimension ref="A1:AI41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y40" sqref="Y40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4986,7 +4986,7 @@
         <v>53</v>
       </c>
       <c r="Y34" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="Z34" s="3" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
fixed statement prime calling wrong statement
</commit_message>
<xml_diff>
--- a/FindDuplicates/PascalParseTable.xlsx
+++ b/FindDuplicates/PascalParseTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin\home\chris\CompilerConstruction\FindDuplicates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3AA629-5FAF-48C1-ABBB-9903339E3990}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80929CD-442F-4FE3-9F50-08387BBA3C77}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="16335" windowHeight="10830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -336,34 +336,6 @@
   <si>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>stmnt stmnt_lst</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <i/>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
@@ -920,6 +892,42 @@
   </si>
   <si>
     <t>subprgrm_head subprgrm_declp</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>stmnt stmnt_lst</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>p</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1351,9 +1359,9 @@
   </sheetPr>
   <dimension ref="A1:AI41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y40" sqref="Y40"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1407,7 +1415,7 @@
         <v>27</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>28</v>
@@ -1446,7 +1454,7 @@
         <v>39</v>
       </c>
       <c r="V1" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W1" s="8" t="s">
         <v>40</v>
@@ -1479,10 +1487,10 @@
         <v>49</v>
       </c>
       <c r="AG1" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH1" s="14" t="s">
         <v>112</v>
-      </c>
-      <c r="AH1" s="14" t="s">
-        <v>113</v>
       </c>
       <c r="AI1" s="10" t="s">
         <v>52</v>
@@ -1493,7 +1501,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>50</v>
@@ -1597,28 +1605,28 @@
     </row>
     <row r="3" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>50</v>
@@ -1654,7 +1662,7 @@
         <v>51</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U3" s="3" t="s">
         <v>50</v>
@@ -1704,7 +1712,7 @@
     </row>
     <row r="4" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>50</v>
@@ -1761,7 +1769,7 @@
         <v>51</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>50</v>
@@ -1817,7 +1825,7 @@
         <v>50</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>50</v>
@@ -1918,7 +1926,7 @@
     </row>
     <row r="6" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>50</v>
@@ -1936,7 +1944,7 @@
         <v>50</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>50</v>
@@ -2046,7 +2054,7 @@
         <v>50</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>50</v>
@@ -2132,7 +2140,7 @@
     </row>
     <row r="8" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>50</v>
@@ -2153,7 +2161,7 @@
         <v>50</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>50</v>
@@ -2507,7 +2515,7 @@
         <v>50</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T11" s="3" t="s">
         <v>50</v>
@@ -2560,7 +2568,7 @@
     </row>
     <row r="12" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>50</v>
@@ -2614,7 +2622,7 @@
         <v>50</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T12" s="11" t="s">
         <v>53</v>
@@ -2721,7 +2729,7 @@
         <v>50</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T13" s="3" t="s">
         <v>50</v>
@@ -2774,28 +2782,28 @@
     </row>
     <row r="14" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>50</v>
@@ -2881,7 +2889,7 @@
     </row>
     <row r="15" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>50</v>
@@ -3042,7 +3050,7 @@
         <v>50</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T16" s="3" t="s">
         <v>50</v>
@@ -3095,7 +3103,7 @@
     </row>
     <row r="17" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>50</v>
@@ -3315,7 +3323,7 @@
         <v>50</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>50</v>
@@ -3416,7 +3424,7 @@
     </row>
     <row r="20" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>50</v>
@@ -3431,7 +3439,7 @@
         <v>53</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>50</v>
@@ -3580,7 +3588,7 @@
         <v>50</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="U21" s="3" t="s">
         <v>50</v>
@@ -3630,7 +3638,7 @@
     </row>
     <row r="22" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>50</v>
@@ -3850,7 +3858,7 @@
         <v>50</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>50</v>
@@ -3901,7 +3909,7 @@
         <v>50</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U24" s="3" t="s">
         <v>50</v>
@@ -3910,7 +3918,7 @@
         <v>50</v>
       </c>
       <c r="W24" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="X24" s="3" t="s">
         <v>50</v>
@@ -3919,13 +3927,13 @@
         <v>50</v>
       </c>
       <c r="Z24" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA24" s="3" t="s">
         <v>50</v>
       </c>
       <c r="AB24" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AC24" s="3" t="s">
         <v>50</v>
@@ -3951,7 +3959,7 @@
     </row>
     <row r="25" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>50</v>
@@ -3966,7 +3974,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>59</v>
+        <v>114</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>50</v>
@@ -4064,7 +4072,7 @@
         <v>50</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>50</v>
@@ -4124,7 +4132,7 @@
         <v>50</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X26" s="3" t="s">
         <v>50</v>
@@ -4133,7 +4141,7 @@
         <v>50</v>
       </c>
       <c r="Z26" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AA26" s="3" t="s">
         <v>50</v>
@@ -4171,7 +4179,7 @@
         <v>50</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>50</v>
@@ -4272,7 +4280,7 @@
     </row>
     <row r="28" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>50</v>
@@ -4305,7 +4313,7 @@
         <v>50</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M28" s="3" t="s">
         <v>50</v>
@@ -4460,7 +4468,7 @@
         <v>50</v>
       </c>
       <c r="AB29" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AC29" s="3" t="s">
         <v>50</v>
@@ -4486,7 +4494,7 @@
     </row>
     <row r="30" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>50</v>
@@ -4495,7 +4503,7 @@
         <v>50</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>50</v>
@@ -4599,10 +4607,10 @@
         <v>50</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>50</v>
@@ -4638,7 +4646,7 @@
         <v>50</v>
       </c>
       <c r="P31" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q31" s="3" t="s">
         <v>50</v>
@@ -4686,13 +4694,13 @@
         <v>50</v>
       </c>
       <c r="AF31" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AG31" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH31" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AI31" s="3" t="s">
         <v>50</v>
@@ -4700,7 +4708,7 @@
     </row>
     <row r="32" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>50</v>
@@ -4718,7 +4726,7 @@
         <v>50</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>50</v>
@@ -4813,10 +4821,10 @@
         <v>50</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>50</v>
@@ -4852,7 +4860,7 @@
         <v>50</v>
       </c>
       <c r="P33" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q33" s="3" t="s">
         <v>50</v>
@@ -4900,13 +4908,13 @@
         <v>50</v>
       </c>
       <c r="AF33" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AG33" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AH33" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AI33" s="3" t="s">
         <v>50</v>
@@ -4914,7 +4922,7 @@
     </row>
     <row r="34" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>50</v>
@@ -4998,7 +5006,7 @@
         <v>50</v>
       </c>
       <c r="AC34" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AD34" s="3" t="s">
         <v>50</v>
@@ -5027,100 +5035,100 @@
         <v>50</v>
       </c>
       <c r="C35" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="N35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P35" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="S35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="U35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="V35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="W35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="X35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF35" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG35" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="AH35" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="K35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="L35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="N35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="O35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P35" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="R35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="S35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="T35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="U35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="V35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="W35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="X35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF35" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="AG35" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="AH35" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="AI35" s="3" t="s">
         <v>50</v>
@@ -5128,7 +5136,7 @@
     </row>
     <row r="36" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>50</v>
@@ -5215,7 +5223,7 @@
         <v>53</v>
       </c>
       <c r="AD36" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AE36" s="3" t="s">
         <v>50</v>
@@ -5241,10 +5249,10 @@
         <v>50</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>50</v>
@@ -5280,7 +5288,7 @@
         <v>50</v>
       </c>
       <c r="P37" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q37" s="3" t="s">
         <v>50</v>
@@ -5328,7 +5336,7 @@
         <v>50</v>
       </c>
       <c r="AF37" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AG37" s="3" t="s">
         <v>50</v>
@@ -5342,7 +5350,7 @@
     </row>
     <row r="38" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>50</v>
@@ -5432,7 +5440,7 @@
         <v>53</v>
       </c>
       <c r="AE38" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AF38" s="3" t="s">
         <v>50</v>
@@ -5455,10 +5463,10 @@
         <v>50</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>50</v>
@@ -5542,7 +5550,7 @@
         <v>50</v>
       </c>
       <c r="AF39" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AG39" s="3" t="s">
         <v>50</v>
@@ -5556,7 +5564,7 @@
     </row>
     <row r="40" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>50</v>
@@ -5589,7 +5597,7 @@
         <v>50</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M40" s="11" t="s">
         <v>53</v>
@@ -5759,10 +5767,10 @@
         <v>50</v>
       </c>
       <c r="AG41" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH41" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="AH41" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="AI41" s="3" t="s">
         <v>50</v>

</xml_diff>